<commit_message>
add methylation correction calculation
</commit_message>
<xml_diff>
--- a/data/PAME_peak_map.xlsx
+++ b/data/PAME_peak_map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tristan/active_repos/tristan_d2o/data/IRMS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sk/Dropbox/Science/manuscripts/20220301 soil growth rates Tristan paper/Caro-et-al.-Soil-Turnover/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D703DE9F-B383-5F4E-BA17-39548B2617FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E02D032-1A06-DE4A-A584-A3280C3E9ADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" xr2:uid="{42725BC7-9775-E54E-AA2D-819F4CD6C3D8}"/>
+    <workbookView xWindow="6220" yWindow="3420" windowWidth="35700" windowHeight="19760" xr2:uid="{42725BC7-9775-E54E-AA2D-819F4CD6C3D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="21">
   <si>
     <t>compound</t>
   </si>
@@ -42,7 +42,61 @@
     <t>PAME</t>
   </si>
   <si>
-    <t>rt</t>
+    <t>peak_type</t>
+  </si>
+  <si>
+    <t>ref_nr</t>
+  </si>
+  <si>
+    <t>calib_peak</t>
+  </si>
+  <si>
+    <t>rt:standard</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>ref</t>
+  </si>
+  <si>
+    <t>analyte</t>
+  </si>
+  <si>
+    <t>C14M</t>
+  </si>
+  <si>
+    <t>iso-std</t>
+  </si>
+  <si>
+    <t>C14E</t>
+  </si>
+  <si>
+    <t>C16M</t>
+  </si>
+  <si>
+    <t>C16E</t>
+  </si>
+  <si>
+    <t>C18M</t>
+  </si>
+  <si>
+    <t>C18E</t>
+  </si>
+  <si>
+    <t>C20M</t>
+  </si>
+  <si>
+    <t>C20E</t>
+  </si>
+  <si>
+    <t>rt:pame</t>
+  </si>
+  <si>
+    <t>hexane</t>
+  </si>
+  <si>
+    <t>solvent</t>
   </si>
 </sst>
 </file>
@@ -78,9 +132,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -99,9 +154,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -139,7 +194,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -245,7 +300,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -387,7 +442,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -395,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68C98B25-6EE0-4840-901A-84A0A10B93FB}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -406,20 +461,476 @@
     <col min="1" max="1" width="14.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="D2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
+        <v>71</v>
+      </c>
+      <c r="F2" s="2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>110</v>
+      </c>
+      <c r="F3" s="2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>150</v>
+      </c>
+      <c r="F4" s="2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>187</v>
+      </c>
+      <c r="F5" s="2">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>226</v>
+      </c>
+      <c r="F6" s="2">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2">
+        <v>270</v>
+      </c>
+      <c r="F7" s="2">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2">
+        <v>310</v>
+      </c>
+      <c r="F8" s="2">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
+        <v>345</v>
+      </c>
+      <c r="F9" s="2">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
+      </c>
+      <c r="D10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2">
+        <v>385</v>
+      </c>
+      <c r="F10" s="2">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2">
+        <v>425</v>
+      </c>
+      <c r="F11" s="2">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <v>11</v>
+      </c>
+      <c r="D12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2">
+        <v>465</v>
+      </c>
+      <c r="F12" s="2">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13">
+        <v>12</v>
+      </c>
+      <c r="D13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2">
+        <v>505</v>
+      </c>
+      <c r="F13" s="2">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="2">
+        <v>643</v>
+      </c>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2">
         <v>745</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="2">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="2">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="2">
+        <v>1170</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="2">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1370</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="2">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="2">
+        <v>1560</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="2">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24">
+        <v>13</v>
+      </c>
+      <c r="D24" t="b">
+        <v>0</v>
+      </c>
+      <c r="E24" s="2">
+        <v>1890</v>
+      </c>
+      <c r="F24" s="2">
+        <v>1890</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25">
+        <v>14</v>
+      </c>
+      <c r="D25" t="b">
+        <v>1</v>
+      </c>
+      <c r="E25" s="2">
+        <v>1930</v>
+      </c>
+      <c r="F25" s="2">
+        <v>1930</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26">
+        <v>15</v>
+      </c>
+      <c r="D26" t="b">
+        <v>0</v>
+      </c>
+      <c r="E26" s="2">
+        <v>1970</v>
+      </c>
+      <c r="F26" s="2">
+        <v>1970</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27">
+        <v>16</v>
+      </c>
+      <c r="D27" t="b">
+        <v>1</v>
+      </c>
+      <c r="E27" s="2">
+        <v>2010</v>
+      </c>
+      <c r="F27" s="2">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28">
+        <v>17</v>
+      </c>
+      <c r="D28" t="b">
+        <v>0</v>
+      </c>
+      <c r="E28" s="2">
+        <v>2050</v>
+      </c>
+      <c r="F28" s="2">
+        <v>2050</v>
       </c>
     </row>
   </sheetData>

</xml_diff>